<commit_message>
make_demand_manual.xlsx file changed, but demand.tss was already good
</commit_message>
<xml_diff>
--- a/input_data/PL/make_demand_manual.xlsx
+++ b/input_data/PL/make_demand_manual.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\verstege\Documents\scripts\local_urbanization\input_data\PL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nauka\Geobazy\CORINE\Student_Assistant_Judith\from_Judith\RegionalUrbanGrowth\RegionalUrbanGrowth\input_data\PL\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
   <si>
     <t>year</t>
   </si>
@@ -53,13 +53,7 @@
     <t>area max (ha)</t>
   </si>
   <si>
-    <t>{'90': 57905.0, '00': 87704.0, '06': 111351.0, '12': 114357.0, '18': 115234.0}</t>
-  </si>
-  <si>
-    <t>{'90': 57905.0, '00': 88495.0, '06': 112356.0, '12': 114909.0, '18': 115410.0}</t>
-  </si>
-  <si>
-    <t>{'90': 57905.0, '00': 88092.0, '06': 111785.0, '12': 114662.0, '18': 115333.0}</t>
+    <t>{'90': 112207.0, '00': 128971.0, '06': 185495.0, '12': 198961.0, '18': 201251.0}</t>
   </si>
 </sst>
 </file>
@@ -107,7 +101,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -125,7 +119,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="pl-PL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -263,91 +257,91 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="29"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>57905</c:v>
+                  <c:v>112207</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>60923.7</c:v>
+                  <c:v>113883.4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>63942.399999999994</c:v>
+                  <c:v>115559.79999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>66961.099999999991</c:v>
+                  <c:v>117236.19999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>69979.799999999988</c:v>
+                  <c:v>118912.59999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>72998.499999999985</c:v>
+                  <c:v>120588.99999999997</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>76017.199999999983</c:v>
+                  <c:v>122265.39999999997</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>79035.89999999998</c:v>
+                  <c:v>123941.79999999996</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>82054.599999999977</c:v>
+                  <c:v>125618.19999999995</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>85073.299999999974</c:v>
+                  <c:v>127294.59999999995</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>88091.999999999971</c:v>
+                  <c:v>128970.99999999994</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>92040.833333333299</c:v>
+                  <c:v>138391.6666666666</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>95989.666666666628</c:v>
+                  <c:v>147812.33333333326</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>99938.499999999956</c:v>
+                  <c:v>157232.99999999991</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>103887.33333333328</c:v>
+                  <c:v>166653.66666666657</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>107836.16666666661</c:v>
+                  <c:v>176074.33333333323</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>111784.99999999994</c:v>
+                  <c:v>185494.99999999988</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>112264.49999999994</c:v>
+                  <c:v>187739.33333333323</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>112743.99999999994</c:v>
+                  <c:v>189983.66666666657</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>113223.49999999994</c:v>
+                  <c:v>192227.99999999991</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>113702.99999999994</c:v>
+                  <c:v>194472.33333333326</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>114182.49999999994</c:v>
+                  <c:v>196716.6666666666</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>114661.99999999994</c:v>
+                  <c:v>198960.99999999994</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>114773.83333333327</c:v>
+                  <c:v>199342.6666666666</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>114885.6666666666</c:v>
+                  <c:v>199724.33333333326</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>114997.49999999993</c:v>
+                  <c:v>200105.99999999991</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>115109.33333333326</c:v>
+                  <c:v>200487.66666666657</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>115221.16666666658</c:v>
+                  <c:v>200869.33333333323</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>115332.99999999991</c:v>
+                  <c:v>201250.99999999988</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -426,19 +420,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>57905</c:v>
+                  <c:v>112207</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>88092</c:v>
+                  <c:v>128971</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>111785</c:v>
+                  <c:v>185495</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>114662</c:v>
+                  <c:v>198961</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>115333</c:v>
+                  <c:v>201251</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -571,91 +565,91 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="29"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>57905</c:v>
+                  <c:v>112207</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>60884.9</c:v>
+                  <c:v>113883.4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>63864.800000000003</c:v>
+                  <c:v>115559.79999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>66844.7</c:v>
+                  <c:v>117236.19999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>69824.599999999991</c:v>
+                  <c:v>118912.59999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>72804.499999999985</c:v>
+                  <c:v>120588.99999999997</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>75784.39999999998</c:v>
+                  <c:v>122265.39999999997</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>78764.299999999974</c:v>
+                  <c:v>123941.79999999996</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>81744.199999999968</c:v>
+                  <c:v>125618.19999999995</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>84724.099999999962</c:v>
+                  <c:v>127294.59999999995</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>87703.999999999956</c:v>
+                  <c:v>128970.99999999994</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>91645.166666666628</c:v>
+                  <c:v>138391.6666666666</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>95586.333333333299</c:v>
+                  <c:v>147812.33333333326</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>99527.499999999971</c:v>
+                  <c:v>157232.99999999991</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>103468.66666666664</c:v>
+                  <c:v>166653.66666666657</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>107409.83333333331</c:v>
+                  <c:v>176074.33333333323</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>111350.99999999999</c:v>
+                  <c:v>185494.99999999988</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>111943.99999999999</c:v>
+                  <c:v>187739.33333333323</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>112536.99999999999</c:v>
+                  <c:v>189983.66666666657</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>113129.99999999999</c:v>
+                  <c:v>192227.99999999991</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>113722.99999999999</c:v>
+                  <c:v>194472.33333333326</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>114315.99999999999</c:v>
+                  <c:v>196716.6666666666</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>114908.99999999999</c:v>
+                  <c:v>198960.99999999994</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>114963.16666666666</c:v>
+                  <c:v>199342.6666666666</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>115017.33333333333</c:v>
+                  <c:v>199724.33333333326</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>115071.5</c:v>
+                  <c:v>200105.99999999991</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>115125.66666666667</c:v>
+                  <c:v>200487.66666666657</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>115179.83333333334</c:v>
+                  <c:v>200869.33333333323</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>115234.00000000001</c:v>
+                  <c:v>201250.99999999988</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -789,91 +783,91 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="29"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>57905</c:v>
+                  <c:v>112207</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>60964</c:v>
+                  <c:v>113883.4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>64023</c:v>
+                  <c:v>115559.79999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>67082</c:v>
+                  <c:v>117236.19999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>70141</c:v>
+                  <c:v>118912.59999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>73200</c:v>
+                  <c:v>120588.99999999997</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>76259</c:v>
+                  <c:v>122265.39999999997</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>79318</c:v>
+                  <c:v>123941.79999999996</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>82377</c:v>
+                  <c:v>125618.19999999995</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>85436</c:v>
+                  <c:v>127294.59999999995</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>88495</c:v>
+                  <c:v>128970.99999999994</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>92471.833333333328</c:v>
+                  <c:v>138391.6666666666</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>96448.666666666657</c:v>
+                  <c:v>147812.33333333326</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>100425.49999999999</c:v>
+                  <c:v>157232.99999999991</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>104402.33333333331</c:v>
+                  <c:v>166653.66666666657</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>108379.16666666664</c:v>
+                  <c:v>176074.33333333323</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>112355.99999999997</c:v>
+                  <c:v>185494.99999999988</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>112689.49999999997</c:v>
+                  <c:v>187739.33333333323</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>113022.99999999997</c:v>
+                  <c:v>189983.66666666657</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>113356.49999999997</c:v>
+                  <c:v>192227.99999999991</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>113689.99999999997</c:v>
+                  <c:v>194472.33333333326</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>114023.49999999997</c:v>
+                  <c:v>196716.6666666666</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>114356.99999999997</c:v>
+                  <c:v>198960.99999999994</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>114532.49999999997</c:v>
+                  <c:v>199342.6666666666</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>114707.99999999997</c:v>
+                  <c:v>199724.33333333326</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>114883.49999999997</c:v>
+                  <c:v>200105.99999999991</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>115058.99999999997</c:v>
+                  <c:v>200487.66666666657</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>115234.49999999997</c:v>
+                  <c:v>200869.33333333323</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>115409.99999999997</c:v>
+                  <c:v>201250.99999999988</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -951,7 +945,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="605890607"/>
@@ -1014,7 +1008,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="605896847"/>
@@ -1055,7 +1049,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="pl-PL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1658,9 +1652,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Pakiet Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1698,7 +1692,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Pakiet Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1770,7 +1764,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Pakiet Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1920,21 +1914,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O32"/>
+  <dimension ref="A1:Q32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1961,32 +1955,31 @@
       </c>
       <c r="K1" s="2"/>
       <c r="L1">
-        <f>B2</f>
-        <v>57905</v>
+        <v>112207</v>
       </c>
       <c r="N1">
         <f>D2</f>
-        <v>57905</v>
+        <v>112207</v>
       </c>
       <c r="O1">
         <f>F2</f>
-        <v>57905</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+        <v>112207</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1990</v>
       </c>
       <c r="B2">
-        <v>57905</v>
+        <v>112207</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2">
-        <v>57905</v>
+        <v>112207</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2">
-        <v>57905</v>
+        <v>112207</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
@@ -1999,41 +1992,45 @@
       </c>
       <c r="L2" s="1">
         <f>B2+C3</f>
-        <v>60923.7</v>
+        <v>113883.4</v>
       </c>
       <c r="N2" s="1">
         <f>D2+E3</f>
-        <v>60884.9</v>
+        <v>113883.4</v>
       </c>
       <c r="O2" s="1">
         <f>F2+G$3</f>
-        <v>60964</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+        <v>113883.4</v>
+      </c>
+      <c r="Q2" s="1">
+        <f>L2-L1</f>
+        <v>1676.3999999999942</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2000</v>
       </c>
       <c r="B3">
-        <v>88092</v>
+        <v>128971</v>
       </c>
       <c r="C3" s="1">
         <f>(B3-B2)/($A3-$A2)</f>
-        <v>3018.7</v>
+        <v>1676.4</v>
       </c>
       <c r="D3">
-        <v>87704</v>
+        <v>128971</v>
       </c>
       <c r="E3" s="1">
         <f>(D3-D2)/($A3-$A2)</f>
-        <v>2979.9</v>
+        <v>1676.4</v>
       </c>
       <c r="F3">
-        <v>88495</v>
+        <v>128971</v>
       </c>
       <c r="G3" s="1">
         <f>(F3-F2)/($A3-$A2)</f>
-        <v>3059</v>
+        <v>1676.4</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -2045,41 +2042,45 @@
       </c>
       <c r="L3" s="1">
         <f t="shared" ref="L3:N11" si="0">L2+C$3</f>
-        <v>63942.399999999994</v>
+        <v>115559.79999999999</v>
       </c>
       <c r="N3" s="1">
         <f>N2+E$3</f>
-        <v>63864.800000000003</v>
+        <v>115559.79999999999</v>
       </c>
       <c r="O3" s="1">
         <f>O2+G$3</f>
-        <v>64023</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+        <v>115559.79999999999</v>
+      </c>
+      <c r="Q3" s="1">
+        <f t="shared" ref="Q3:Q29" si="1">L3-L2</f>
+        <v>1676.3999999999942</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2006</v>
       </c>
       <c r="B4">
-        <v>111785</v>
+        <v>185495</v>
       </c>
       <c r="C4" s="1">
-        <f t="shared" ref="C4:G5" si="1">(B4-B3)/($A4-$A3)</f>
-        <v>3948.8333333333335</v>
+        <f t="shared" ref="C4:G5" si="2">(B4-B3)/($A4-$A3)</f>
+        <v>9420.6666666666661</v>
       </c>
       <c r="D4">
-        <v>111351</v>
+        <v>185495</v>
       </c>
       <c r="E4" s="1">
-        <f t="shared" si="1"/>
-        <v>3941.1666666666665</v>
+        <f t="shared" si="2"/>
+        <v>9420.6666666666661</v>
       </c>
       <c r="F4">
-        <v>112356</v>
+        <v>185495</v>
       </c>
       <c r="G4" s="1">
-        <f t="shared" si="1"/>
-        <v>3976.8333333333335</v>
+        <f t="shared" si="2"/>
+        <v>9420.6666666666661</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -2091,41 +2092,45 @@
       </c>
       <c r="L4" s="1">
         <f t="shared" si="0"/>
-        <v>66961.099999999991</v>
+        <v>117236.19999999998</v>
       </c>
       <c r="N4" s="1">
         <f t="shared" si="0"/>
-        <v>66844.7</v>
+        <v>117236.19999999998</v>
       </c>
       <c r="O4" s="1">
-        <f t="shared" ref="O4:O11" si="2">O3+G$3</f>
-        <v>67082</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+        <f t="shared" ref="O4:O11" si="3">O3+G$3</f>
+        <v>117236.19999999998</v>
+      </c>
+      <c r="Q4" s="1">
+        <f t="shared" si="1"/>
+        <v>1676.3999999999942</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2012</v>
       </c>
       <c r="B5">
-        <v>114662</v>
+        <v>198961</v>
       </c>
       <c r="C5" s="1">
-        <f t="shared" si="1"/>
-        <v>479.5</v>
+        <f t="shared" si="2"/>
+        <v>2244.3333333333335</v>
       </c>
       <c r="D5">
-        <v>114909</v>
+        <v>198961</v>
       </c>
       <c r="E5" s="1">
-        <f t="shared" si="1"/>
-        <v>593</v>
+        <f t="shared" si="2"/>
+        <v>2244.3333333333335</v>
       </c>
       <c r="F5">
-        <v>114357</v>
+        <v>198961</v>
       </c>
       <c r="G5" s="1">
-        <f t="shared" si="1"/>
-        <v>333.5</v>
+        <f t="shared" si="2"/>
+        <v>2244.3333333333335</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -2137,41 +2142,45 @@
       </c>
       <c r="L5" s="1">
         <f t="shared" si="0"/>
-        <v>69979.799999999988</v>
+        <v>118912.59999999998</v>
       </c>
       <c r="N5" s="1">
         <f t="shared" si="0"/>
-        <v>69824.599999999991</v>
+        <v>118912.59999999998</v>
       </c>
       <c r="O5" s="1">
-        <f t="shared" si="2"/>
-        <v>70141</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>118912.59999999998</v>
+      </c>
+      <c r="Q5" s="1">
+        <f t="shared" si="1"/>
+        <v>1676.3999999999942</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2018</v>
       </c>
       <c r="B6">
-        <v>115333</v>
+        <v>201251</v>
       </c>
       <c r="C6" s="1">
         <f>(B6-B5)/($A6-$A5)</f>
-        <v>111.83333333333333</v>
+        <v>381.66666666666669</v>
       </c>
       <c r="D6">
-        <v>115234</v>
+        <v>201251</v>
       </c>
       <c r="E6" s="1">
         <f>(D6-D5)/($A6-$A5)</f>
-        <v>54.166666666666664</v>
+        <v>381.66666666666669</v>
       </c>
       <c r="F6">
-        <v>115410</v>
+        <v>201251</v>
       </c>
       <c r="G6" s="1">
         <f>(F6-F5)/($A6-$A5)</f>
-        <v>175.5</v>
+        <v>381.66666666666669</v>
       </c>
       <c r="J6">
         <v>1995</v>
@@ -2181,18 +2190,22 @@
       </c>
       <c r="L6" s="1">
         <f t="shared" si="0"/>
-        <v>72998.499999999985</v>
+        <v>120588.99999999997</v>
       </c>
       <c r="N6" s="1">
         <f t="shared" si="0"/>
-        <v>72804.499999999985</v>
+        <v>120588.99999999997</v>
       </c>
       <c r="O6" s="1">
-        <f t="shared" si="2"/>
-        <v>73200</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>120588.99999999997</v>
+      </c>
+      <c r="Q6" s="1">
+        <f t="shared" si="1"/>
+        <v>1676.3999999999942</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="J7">
         <v>1996</v>
       </c>
@@ -2201,18 +2214,22 @@
       </c>
       <c r="L7" s="1">
         <f t="shared" si="0"/>
-        <v>76017.199999999983</v>
+        <v>122265.39999999997</v>
       </c>
       <c r="N7" s="1">
         <f t="shared" si="0"/>
-        <v>75784.39999999998</v>
+        <v>122265.39999999997</v>
       </c>
       <c r="O7" s="1">
-        <f t="shared" si="2"/>
-        <v>76259</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>122265.39999999997</v>
+      </c>
+      <c r="Q7" s="1">
+        <f t="shared" si="1"/>
+        <v>1676.3999999999942</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="J8">
         <v>1997</v>
       </c>
@@ -2221,18 +2238,22 @@
       </c>
       <c r="L8" s="1">
         <f t="shared" si="0"/>
-        <v>79035.89999999998</v>
+        <v>123941.79999999996</v>
       </c>
       <c r="N8" s="1">
         <f t="shared" si="0"/>
-        <v>78764.299999999974</v>
+        <v>123941.79999999996</v>
       </c>
       <c r="O8" s="1">
-        <f t="shared" si="2"/>
-        <v>79318</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>123941.79999999996</v>
+      </c>
+      <c r="Q8" s="1">
+        <f t="shared" si="1"/>
+        <v>1676.3999999999942</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="J9">
         <v>1998</v>
       </c>
@@ -2240,19 +2261,23 @@
         <v>8</v>
       </c>
       <c r="L9" s="1">
-        <f t="shared" si="0"/>
-        <v>82054.599999999977</v>
+        <f>L8+C$3</f>
+        <v>125618.19999999995</v>
       </c>
       <c r="N9" s="1">
         <f t="shared" si="0"/>
-        <v>81744.199999999968</v>
+        <v>125618.19999999995</v>
       </c>
       <c r="O9" s="1">
-        <f t="shared" si="2"/>
-        <v>82377</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>125618.19999999995</v>
+      </c>
+      <c r="Q9" s="1">
+        <f t="shared" si="1"/>
+        <v>1676.3999999999942</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="J10">
         <v>1999</v>
       </c>
@@ -2261,18 +2286,22 @@
       </c>
       <c r="L10" s="1">
         <f t="shared" si="0"/>
-        <v>85073.299999999974</v>
+        <v>127294.59999999995</v>
       </c>
       <c r="N10" s="1">
         <f t="shared" si="0"/>
-        <v>84724.099999999962</v>
+        <v>127294.59999999995</v>
       </c>
       <c r="O10" s="1">
-        <f t="shared" si="2"/>
-        <v>85436</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>127294.59999999995</v>
+      </c>
+      <c r="Q10" s="1">
+        <f t="shared" si="1"/>
+        <v>1676.3999999999942</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="J11">
         <v>2000</v>
       </c>
@@ -2281,18 +2310,22 @@
       </c>
       <c r="L11" s="1">
         <f t="shared" si="0"/>
-        <v>88091.999999999971</v>
+        <v>128970.99999999994</v>
       </c>
       <c r="N11" s="1">
         <f t="shared" si="0"/>
-        <v>87703.999999999956</v>
+        <v>128970.99999999994</v>
       </c>
       <c r="O11" s="1">
-        <f t="shared" si="2"/>
-        <v>88495</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>128970.99999999994</v>
+      </c>
+      <c r="Q11" s="1">
+        <f t="shared" si="1"/>
+        <v>1676.3999999999942</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="J12">
         <v>2001</v>
       </c>
@@ -2301,18 +2334,22 @@
       </c>
       <c r="L12" s="1">
         <f>L11+C$4</f>
-        <v>92040.833333333299</v>
+        <v>138391.6666666666</v>
       </c>
       <c r="N12" s="1">
         <f>N11+E$4</f>
-        <v>91645.166666666628</v>
+        <v>138391.6666666666</v>
       </c>
       <c r="O12" s="1">
         <f>O11+G$4</f>
-        <v>92471.833333333328</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+        <v>138391.6666666666</v>
+      </c>
+      <c r="Q12" s="1">
+        <f t="shared" si="1"/>
+        <v>9420.666666666657</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="J13">
         <v>2002</v>
       </c>
@@ -2320,19 +2357,23 @@
         <v>12</v>
       </c>
       <c r="L13" s="1">
-        <f t="shared" ref="L13:N17" si="3">L12+C$4</f>
-        <v>95989.666666666628</v>
+        <f t="shared" ref="L13:N17" si="4">L12+C$4</f>
+        <v>147812.33333333326</v>
       </c>
       <c r="N13" s="1">
-        <f t="shared" si="3"/>
-        <v>95586.333333333299</v>
+        <f t="shared" si="4"/>
+        <v>147812.33333333326</v>
       </c>
       <c r="O13" s="1">
-        <f t="shared" ref="O13:O17" si="4">O12+G$4</f>
-        <v>96448.666666666657</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+        <f t="shared" ref="O13:O17" si="5">O12+G$4</f>
+        <v>147812.33333333326</v>
+      </c>
+      <c r="Q13" s="1">
+        <f t="shared" si="1"/>
+        <v>9420.666666666657</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="J14">
         <v>2003</v>
       </c>
@@ -2340,19 +2381,23 @@
         <v>13</v>
       </c>
       <c r="L14" s="1">
-        <f t="shared" si="3"/>
-        <v>99938.499999999956</v>
+        <f t="shared" si="4"/>
+        <v>157232.99999999991</v>
       </c>
       <c r="N14" s="1">
-        <f t="shared" si="3"/>
-        <v>99527.499999999971</v>
+        <f t="shared" si="4"/>
+        <v>157232.99999999991</v>
       </c>
       <c r="O14" s="1">
-        <f t="shared" si="4"/>
-        <v>100425.49999999999</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+        <f t="shared" si="5"/>
+        <v>157232.99999999991</v>
+      </c>
+      <c r="Q14" s="1">
+        <f t="shared" si="1"/>
+        <v>9420.666666666657</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="J15">
         <v>2004</v>
       </c>
@@ -2360,19 +2405,23 @@
         <v>14</v>
       </c>
       <c r="L15" s="1">
-        <f t="shared" si="3"/>
-        <v>103887.33333333328</v>
+        <f t="shared" si="4"/>
+        <v>166653.66666666657</v>
       </c>
       <c r="N15" s="1">
-        <f t="shared" si="3"/>
-        <v>103468.66666666664</v>
+        <f t="shared" si="4"/>
+        <v>166653.66666666657</v>
       </c>
       <c r="O15" s="1">
-        <f t="shared" si="4"/>
-        <v>104402.33333333331</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+        <f t="shared" si="5"/>
+        <v>166653.66666666657</v>
+      </c>
+      <c r="Q15" s="1">
+        <f t="shared" si="1"/>
+        <v>9420.666666666657</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="J16">
         <v>2005</v>
       </c>
@@ -2380,19 +2429,23 @@
         <v>15</v>
       </c>
       <c r="L16" s="1">
-        <f t="shared" si="3"/>
-        <v>107836.16666666661</v>
+        <f t="shared" si="4"/>
+        <v>176074.33333333323</v>
       </c>
       <c r="N16" s="1">
-        <f t="shared" si="3"/>
-        <v>107409.83333333331</v>
+        <f t="shared" si="4"/>
+        <v>176074.33333333323</v>
       </c>
       <c r="O16" s="1">
-        <f t="shared" si="4"/>
-        <v>108379.16666666664</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+        <f t="shared" si="5"/>
+        <v>176074.33333333323</v>
+      </c>
+      <c r="Q16" s="1">
+        <f t="shared" si="1"/>
+        <v>9420.666666666657</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="J17">
         <v>2006</v>
       </c>
@@ -2400,19 +2453,23 @@
         <v>16</v>
       </c>
       <c r="L17" s="1">
-        <f t="shared" si="3"/>
-        <v>111784.99999999994</v>
+        <f t="shared" si="4"/>
+        <v>185494.99999999988</v>
       </c>
       <c r="N17" s="1">
-        <f t="shared" si="3"/>
-        <v>111350.99999999999</v>
+        <f t="shared" si="4"/>
+        <v>185494.99999999988</v>
       </c>
       <c r="O17" s="1">
-        <f t="shared" si="4"/>
-        <v>112355.99999999997</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+        <f t="shared" si="5"/>
+        <v>185494.99999999988</v>
+      </c>
+      <c r="Q17" s="1">
+        <f t="shared" si="1"/>
+        <v>9420.666666666657</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="J18">
         <v>2007</v>
       </c>
@@ -2421,18 +2478,22 @@
       </c>
       <c r="L18" s="1">
         <f>L17+C$5</f>
-        <v>112264.49999999994</v>
+        <v>187739.33333333323</v>
       </c>
       <c r="N18" s="1">
         <f>N17+E$5</f>
-        <v>111943.99999999999</v>
+        <v>187739.33333333323</v>
       </c>
       <c r="O18" s="1">
         <f>O17+G$5</f>
-        <v>112689.49999999997</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+        <v>187739.33333333323</v>
+      </c>
+      <c r="Q18" s="1">
+        <f t="shared" si="1"/>
+        <v>2244.333333333343</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="J19">
         <v>2008</v>
       </c>
@@ -2440,19 +2501,23 @@
         <v>18</v>
       </c>
       <c r="L19" s="1">
-        <f t="shared" ref="L19:N22" si="5">L18+C$5</f>
-        <v>112743.99999999994</v>
+        <f t="shared" ref="L19:N22" si="6">L18+C$5</f>
+        <v>189983.66666666657</v>
       </c>
       <c r="N19" s="1">
-        <f t="shared" si="5"/>
-        <v>112536.99999999999</v>
+        <f t="shared" si="6"/>
+        <v>189983.66666666657</v>
       </c>
       <c r="O19" s="1">
-        <f t="shared" ref="O19:O23" si="6">O18+G$5</f>
-        <v>113022.99999999997</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+        <f t="shared" ref="O19:O23" si="7">O18+G$5</f>
+        <v>189983.66666666657</v>
+      </c>
+      <c r="Q19" s="1">
+        <f t="shared" si="1"/>
+        <v>2244.333333333343</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="J20">
         <v>2009</v>
       </c>
@@ -2460,19 +2525,23 @@
         <v>19</v>
       </c>
       <c r="L20" s="1">
-        <f t="shared" si="5"/>
-        <v>113223.49999999994</v>
+        <f t="shared" si="6"/>
+        <v>192227.99999999991</v>
       </c>
       <c r="N20" s="1">
-        <f t="shared" si="5"/>
-        <v>113129.99999999999</v>
+        <f t="shared" si="6"/>
+        <v>192227.99999999991</v>
       </c>
       <c r="O20" s="1">
-        <f t="shared" si="6"/>
-        <v>113356.49999999997</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+        <f t="shared" si="7"/>
+        <v>192227.99999999991</v>
+      </c>
+      <c r="Q20" s="1">
+        <f t="shared" si="1"/>
+        <v>2244.333333333343</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="J21">
         <v>2010</v>
       </c>
@@ -2480,19 +2549,23 @@
         <v>20</v>
       </c>
       <c r="L21" s="1">
-        <f t="shared" si="5"/>
-        <v>113702.99999999994</v>
+        <f t="shared" si="6"/>
+        <v>194472.33333333326</v>
       </c>
       <c r="N21" s="1">
-        <f t="shared" si="5"/>
-        <v>113722.99999999999</v>
+        <f t="shared" si="6"/>
+        <v>194472.33333333326</v>
       </c>
       <c r="O21" s="1">
-        <f t="shared" si="6"/>
-        <v>113689.99999999997</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+        <f t="shared" si="7"/>
+        <v>194472.33333333326</v>
+      </c>
+      <c r="Q21" s="1">
+        <f t="shared" si="1"/>
+        <v>2244.333333333343</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="J22">
         <v>2011</v>
       </c>
@@ -2500,19 +2573,23 @@
         <v>21</v>
       </c>
       <c r="L22" s="1">
-        <f t="shared" si="5"/>
-        <v>114182.49999999994</v>
+        <f t="shared" si="6"/>
+        <v>196716.6666666666</v>
       </c>
       <c r="N22" s="1">
-        <f t="shared" si="5"/>
-        <v>114315.99999999999</v>
+        <f t="shared" si="6"/>
+        <v>196716.6666666666</v>
       </c>
       <c r="O22" s="1">
-        <f t="shared" si="6"/>
-        <v>114023.49999999997</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+        <f t="shared" si="7"/>
+        <v>196716.6666666666</v>
+      </c>
+      <c r="Q22" s="1">
+        <f t="shared" si="1"/>
+        <v>2244.333333333343</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="J23">
         <v>2012</v>
       </c>
@@ -2521,18 +2598,22 @@
       </c>
       <c r="L23" s="1">
         <f>L22+C$5</f>
-        <v>114661.99999999994</v>
+        <v>198960.99999999994</v>
       </c>
       <c r="N23" s="1">
         <f>N22+E$5</f>
-        <v>114908.99999999999</v>
+        <v>198960.99999999994</v>
       </c>
       <c r="O23" s="1">
-        <f t="shared" si="6"/>
-        <v>114356.99999999997</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+        <f t="shared" si="7"/>
+        <v>198960.99999999994</v>
+      </c>
+      <c r="Q23" s="1">
+        <f t="shared" si="1"/>
+        <v>2244.333333333343</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>6</v>
       </c>
@@ -2547,18 +2628,22 @@
       </c>
       <c r="L24" s="1">
         <f>L23+C$6</f>
-        <v>114773.83333333327</v>
+        <v>199342.6666666666</v>
       </c>
       <c r="N24" s="1">
         <f>N23+E$6</f>
-        <v>114963.16666666666</v>
+        <v>199342.6666666666</v>
       </c>
       <c r="O24" s="1">
         <f>O23+G$6</f>
-        <v>114532.49999999997</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+        <v>199342.6666666666</v>
+      </c>
+      <c r="Q24" s="1">
+        <f t="shared" si="1"/>
+        <v>381.66666666665697</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>3</v>
       </c>
@@ -2573,18 +2658,22 @@
       </c>
       <c r="L25" s="1">
         <f>L24+C$6</f>
-        <v>114885.6666666666</v>
+        <v>199724.33333333326</v>
       </c>
       <c r="N25" s="1">
         <f>N24+E$6</f>
-        <v>115017.33333333333</v>
+        <v>199724.33333333326</v>
       </c>
       <c r="O25" s="1">
         <f>O24+G$6</f>
-        <v>114707.99999999997</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+        <v>199724.33333333326</v>
+      </c>
+      <c r="Q25" s="1">
+        <f t="shared" si="1"/>
+        <v>381.66666666665697</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>4</v>
       </c>
@@ -2598,25 +2687,26 @@
         <v>25</v>
       </c>
       <c r="L26" s="1">
-        <f t="shared" ref="L26:L29" si="7">L25+C$6</f>
-        <v>114997.49999999993</v>
+        <f t="shared" ref="L26:L29" si="8">L25+C$6</f>
+        <v>200105.99999999991</v>
       </c>
       <c r="N26" s="1">
-        <f t="shared" ref="N26:N29" si="8">N25+E$6</f>
-        <v>115071.5</v>
+        <f t="shared" ref="N26:N29" si="9">N25+E$6</f>
+        <v>200105.99999999991</v>
       </c>
       <c r="O26" s="1">
-        <f t="shared" ref="O26:O29" si="9">O25+G$6</f>
-        <v>114883.49999999997</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+        <f t="shared" ref="O26:O29" si="10">O25+G$6</f>
+        <v>200105.99999999991</v>
+      </c>
+      <c r="Q26" s="1">
+        <f t="shared" si="1"/>
+        <v>381.66666666665697</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>5</v>
       </c>
-      <c r="B27" t="s">
-        <v>10</v>
-      </c>
       <c r="J27">
         <v>2016</v>
       </c>
@@ -2624,22 +2714,23 @@
         <v>26</v>
       </c>
       <c r="L27" s="1">
-        <f t="shared" si="7"/>
-        <v>115109.33333333326</v>
+        <f t="shared" si="8"/>
+        <v>200487.66666666657</v>
       </c>
       <c r="N27" s="1">
-        <f t="shared" si="8"/>
-        <v>115125.66666666667</v>
+        <f t="shared" si="9"/>
+        <v>200487.66666666657</v>
       </c>
       <c r="O27" s="1">
-        <f t="shared" si="9"/>
-        <v>115058.99999999997</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B28" t="s">
-        <v>11</v>
-      </c>
+        <f t="shared" si="10"/>
+        <v>200487.66666666657</v>
+      </c>
+      <c r="Q27" s="1">
+        <f t="shared" si="1"/>
+        <v>381.66666666665697</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="J28">
         <v>2017</v>
       </c>
@@ -2647,19 +2738,23 @@
         <v>27</v>
       </c>
       <c r="L28" s="1">
-        <f t="shared" si="7"/>
-        <v>115221.16666666658</v>
+        <f t="shared" si="8"/>
+        <v>200869.33333333323</v>
       </c>
       <c r="N28" s="1">
-        <f t="shared" si="8"/>
-        <v>115179.83333333334</v>
+        <f t="shared" si="9"/>
+        <v>200869.33333333323</v>
       </c>
       <c r="O28" s="1">
-        <f t="shared" si="9"/>
-        <v>115234.49999999997</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+        <f t="shared" si="10"/>
+        <v>200869.33333333323</v>
+      </c>
+      <c r="Q28" s="1">
+        <f t="shared" si="1"/>
+        <v>381.66666666665697</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>6</v>
       </c>
@@ -2670,29 +2765,33 @@
         <v>28</v>
       </c>
       <c r="L29" s="1">
-        <f t="shared" si="7"/>
-        <v>115332.99999999991</v>
+        <f t="shared" si="8"/>
+        <v>201250.99999999988</v>
       </c>
       <c r="N29" s="1">
-        <f t="shared" si="8"/>
-        <v>115234.00000000001</v>
+        <f t="shared" si="9"/>
+        <v>201250.99999999988</v>
       </c>
       <c r="O29" s="1">
-        <f t="shared" si="9"/>
-        <v>115409.99999999997</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+        <f t="shared" si="10"/>
+        <v>201250.99999999988</v>
+      </c>
+      <c r="Q29" s="1">
+        <f t="shared" si="1"/>
+        <v>381.66666666665697</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
1990 as timestep 1 (before as timestep 0)
</commit_message>
<xml_diff>
--- a/input_data/PL/make_demand_manual.xlsx
+++ b/input_data/PL/make_demand_manual.xlsx
@@ -95,10 +95,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -1917,7 +1918,7 @@
   <dimension ref="A1:Q32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="T1" sqref="T1:U31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1953,7 +1954,9 @@
       <c r="J1">
         <v>1990</v>
       </c>
-      <c r="K1" s="2"/>
+      <c r="K1">
+        <v>1</v>
+      </c>
       <c r="L1">
         <v>112207</v>
       </c>
@@ -1988,7 +1991,7 @@
         <v>1991</v>
       </c>
       <c r="K2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L2" s="1">
         <f>B2+C3</f>
@@ -2038,7 +2041,7 @@
         <v>1992</v>
       </c>
       <c r="K3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L3" s="1">
         <f t="shared" ref="L3:N11" si="0">L2+C$3</f>
@@ -2053,7 +2056,7 @@
         <v>115559.79999999999</v>
       </c>
       <c r="Q3" s="1">
-        <f t="shared" ref="Q3:Q29" si="1">L3-L2</f>
+        <f>L3-L2</f>
         <v>1676.3999999999942</v>
       </c>
     </row>
@@ -2065,21 +2068,21 @@
         <v>185495</v>
       </c>
       <c r="C4" s="1">
-        <f t="shared" ref="C4:G5" si="2">(B4-B3)/($A4-$A3)</f>
+        <f t="shared" ref="C4:G5" si="1">(B4-B3)/($A4-$A3)</f>
         <v>9420.6666666666661</v>
       </c>
       <c r="D4">
         <v>185495</v>
       </c>
       <c r="E4" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>9420.6666666666661</v>
       </c>
       <c r="F4">
         <v>185495</v>
       </c>
       <c r="G4" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>9420.6666666666661</v>
       </c>
       <c r="H4" s="1"/>
@@ -2088,7 +2091,7 @@
         <v>1993</v>
       </c>
       <c r="K4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L4" s="1">
         <f t="shared" si="0"/>
@@ -2099,11 +2102,11 @@
         <v>117236.19999999998</v>
       </c>
       <c r="O4" s="1">
-        <f t="shared" ref="O4:O11" si="3">O3+G$3</f>
+        <f t="shared" ref="O4:O11" si="2">O3+G$3</f>
         <v>117236.19999999998</v>
       </c>
       <c r="Q4" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="Q3:Q29" si="3">L4-L3</f>
         <v>1676.3999999999942</v>
       </c>
     </row>
@@ -2115,21 +2118,21 @@
         <v>198961</v>
       </c>
       <c r="C5" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2244.3333333333335</v>
       </c>
       <c r="D5">
         <v>198961</v>
       </c>
       <c r="E5" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2244.3333333333335</v>
       </c>
       <c r="F5">
         <v>198961</v>
       </c>
       <c r="G5" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2244.3333333333335</v>
       </c>
       <c r="H5" s="1"/>
@@ -2138,7 +2141,7 @@
         <v>1994</v>
       </c>
       <c r="K5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L5" s="1">
         <f t="shared" si="0"/>
@@ -2149,11 +2152,11 @@
         <v>118912.59999999998</v>
       </c>
       <c r="O5" s="1">
+        <f t="shared" si="2"/>
+        <v>118912.59999999998</v>
+      </c>
+      <c r="Q5" s="1">
         <f t="shared" si="3"/>
-        <v>118912.59999999998</v>
-      </c>
-      <c r="Q5" s="1">
-        <f t="shared" si="1"/>
         <v>1676.3999999999942</v>
       </c>
     </row>
@@ -2186,7 +2189,7 @@
         <v>1995</v>
       </c>
       <c r="K6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L6" s="1">
         <f t="shared" si="0"/>
@@ -2197,11 +2200,11 @@
         <v>120588.99999999997</v>
       </c>
       <c r="O6" s="1">
+        <f t="shared" si="2"/>
+        <v>120588.99999999997</v>
+      </c>
+      <c r="Q6" s="1">
         <f t="shared" si="3"/>
-        <v>120588.99999999997</v>
-      </c>
-      <c r="Q6" s="1">
-        <f t="shared" si="1"/>
         <v>1676.3999999999942</v>
       </c>
     </row>
@@ -2210,7 +2213,7 @@
         <v>1996</v>
       </c>
       <c r="K7">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L7" s="1">
         <f t="shared" si="0"/>
@@ -2221,11 +2224,11 @@
         <v>122265.39999999997</v>
       </c>
       <c r="O7" s="1">
+        <f t="shared" si="2"/>
+        <v>122265.39999999997</v>
+      </c>
+      <c r="Q7" s="1">
         <f t="shared" si="3"/>
-        <v>122265.39999999997</v>
-      </c>
-      <c r="Q7" s="1">
-        <f t="shared" si="1"/>
         <v>1676.3999999999942</v>
       </c>
     </row>
@@ -2233,8 +2236,8 @@
       <c r="J8">
         <v>1997</v>
       </c>
-      <c r="K8">
-        <v>7</v>
+      <c r="K8" s="3">
+        <v>8</v>
       </c>
       <c r="L8" s="1">
         <f t="shared" si="0"/>
@@ -2245,11 +2248,11 @@
         <v>123941.79999999996</v>
       </c>
       <c r="O8" s="1">
+        <f t="shared" si="2"/>
+        <v>123941.79999999996</v>
+      </c>
+      <c r="Q8" s="1">
         <f t="shared" si="3"/>
-        <v>123941.79999999996</v>
-      </c>
-      <c r="Q8" s="1">
-        <f t="shared" si="1"/>
         <v>1676.3999999999942</v>
       </c>
     </row>
@@ -2257,8 +2260,8 @@
       <c r="J9">
         <v>1998</v>
       </c>
-      <c r="K9">
-        <v>8</v>
+      <c r="K9" s="3">
+        <v>9</v>
       </c>
       <c r="L9" s="1">
         <f>L8+C$3</f>
@@ -2269,11 +2272,11 @@
         <v>125618.19999999995</v>
       </c>
       <c r="O9" s="1">
+        <f t="shared" si="2"/>
+        <v>125618.19999999995</v>
+      </c>
+      <c r="Q9" s="1">
         <f t="shared" si="3"/>
-        <v>125618.19999999995</v>
-      </c>
-      <c r="Q9" s="1">
-        <f t="shared" si="1"/>
         <v>1676.3999999999942</v>
       </c>
     </row>
@@ -2281,8 +2284,8 @@
       <c r="J10">
         <v>1999</v>
       </c>
-      <c r="K10">
-        <v>9</v>
+      <c r="K10" s="3">
+        <v>10</v>
       </c>
       <c r="L10" s="1">
         <f t="shared" si="0"/>
@@ -2293,11 +2296,11 @@
         <v>127294.59999999995</v>
       </c>
       <c r="O10" s="1">
+        <f t="shared" si="2"/>
+        <v>127294.59999999995</v>
+      </c>
+      <c r="Q10" s="1">
         <f t="shared" si="3"/>
-        <v>127294.59999999995</v>
-      </c>
-      <c r="Q10" s="1">
-        <f t="shared" si="1"/>
         <v>1676.3999999999942</v>
       </c>
     </row>
@@ -2306,7 +2309,7 @@
         <v>2000</v>
       </c>
       <c r="K11" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="L11" s="1">
         <f t="shared" si="0"/>
@@ -2317,11 +2320,11 @@
         <v>128970.99999999994</v>
       </c>
       <c r="O11" s="1">
+        <f t="shared" si="2"/>
+        <v>128970.99999999994</v>
+      </c>
+      <c r="Q11" s="1">
         <f t="shared" si="3"/>
-        <v>128970.99999999994</v>
-      </c>
-      <c r="Q11" s="1">
-        <f t="shared" si="1"/>
         <v>1676.3999999999942</v>
       </c>
     </row>
@@ -2329,8 +2332,8 @@
       <c r="J12">
         <v>2001</v>
       </c>
-      <c r="K12">
-        <v>11</v>
+      <c r="K12" s="3">
+        <v>12</v>
       </c>
       <c r="L12" s="1">
         <f>L11+C$4</f>
@@ -2345,7 +2348,7 @@
         <v>138391.6666666666</v>
       </c>
       <c r="Q12" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>9420.666666666657</v>
       </c>
     </row>
@@ -2353,8 +2356,8 @@
       <c r="J13">
         <v>2002</v>
       </c>
-      <c r="K13">
-        <v>12</v>
+      <c r="K13" s="3">
+        <v>13</v>
       </c>
       <c r="L13" s="1">
         <f t="shared" ref="L13:N17" si="4">L12+C$4</f>
@@ -2369,7 +2372,7 @@
         <v>147812.33333333326</v>
       </c>
       <c r="Q13" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>9420.666666666657</v>
       </c>
     </row>
@@ -2377,8 +2380,8 @@
       <c r="J14">
         <v>2003</v>
       </c>
-      <c r="K14">
-        <v>13</v>
+      <c r="K14" s="3">
+        <v>14</v>
       </c>
       <c r="L14" s="1">
         <f t="shared" si="4"/>
@@ -2393,7 +2396,7 @@
         <v>157232.99999999991</v>
       </c>
       <c r="Q14" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>9420.666666666657</v>
       </c>
     </row>
@@ -2401,8 +2404,8 @@
       <c r="J15">
         <v>2004</v>
       </c>
-      <c r="K15">
-        <v>14</v>
+      <c r="K15" s="3">
+        <v>15</v>
       </c>
       <c r="L15" s="1">
         <f t="shared" si="4"/>
@@ -2417,7 +2420,7 @@
         <v>166653.66666666657</v>
       </c>
       <c r="Q15" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>9420.666666666657</v>
       </c>
     </row>
@@ -2425,8 +2428,8 @@
       <c r="J16">
         <v>2005</v>
       </c>
-      <c r="K16">
-        <v>15</v>
+      <c r="K16" s="3">
+        <v>16</v>
       </c>
       <c r="L16" s="1">
         <f t="shared" si="4"/>
@@ -2441,7 +2444,7 @@
         <v>176074.33333333323</v>
       </c>
       <c r="Q16" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>9420.666666666657</v>
       </c>
     </row>
@@ -2450,7 +2453,7 @@
         <v>2006</v>
       </c>
       <c r="K17" s="2">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L17" s="1">
         <f t="shared" si="4"/>
@@ -2465,7 +2468,7 @@
         <v>185494.99999999988</v>
       </c>
       <c r="Q17" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>9420.666666666657</v>
       </c>
     </row>
@@ -2473,8 +2476,8 @@
       <c r="J18">
         <v>2007</v>
       </c>
-      <c r="K18">
-        <v>17</v>
+      <c r="K18" s="3">
+        <v>18</v>
       </c>
       <c r="L18" s="1">
         <f>L17+C$5</f>
@@ -2489,7 +2492,7 @@
         <v>187739.33333333323</v>
       </c>
       <c r="Q18" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2244.333333333343</v>
       </c>
     </row>
@@ -2497,8 +2500,8 @@
       <c r="J19">
         <v>2008</v>
       </c>
-      <c r="K19">
-        <v>18</v>
+      <c r="K19" s="3">
+        <v>19</v>
       </c>
       <c r="L19" s="1">
         <f t="shared" ref="L19:N22" si="6">L18+C$5</f>
@@ -2513,7 +2516,7 @@
         <v>189983.66666666657</v>
       </c>
       <c r="Q19" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2244.333333333343</v>
       </c>
     </row>
@@ -2521,8 +2524,8 @@
       <c r="J20">
         <v>2009</v>
       </c>
-      <c r="K20">
-        <v>19</v>
+      <c r="K20" s="3">
+        <v>20</v>
       </c>
       <c r="L20" s="1">
         <f t="shared" si="6"/>
@@ -2537,7 +2540,7 @@
         <v>192227.99999999991</v>
       </c>
       <c r="Q20" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2244.333333333343</v>
       </c>
     </row>
@@ -2545,8 +2548,8 @@
       <c r="J21">
         <v>2010</v>
       </c>
-      <c r="K21">
-        <v>20</v>
+      <c r="K21" s="3">
+        <v>21</v>
       </c>
       <c r="L21" s="1">
         <f t="shared" si="6"/>
@@ -2561,7 +2564,7 @@
         <v>194472.33333333326</v>
       </c>
       <c r="Q21" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2244.333333333343</v>
       </c>
     </row>
@@ -2569,8 +2572,8 @@
       <c r="J22">
         <v>2011</v>
       </c>
-      <c r="K22">
-        <v>21</v>
+      <c r="K22" s="3">
+        <v>22</v>
       </c>
       <c r="L22" s="1">
         <f t="shared" si="6"/>
@@ -2585,7 +2588,7 @@
         <v>196716.6666666666</v>
       </c>
       <c r="Q22" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2244.333333333343</v>
       </c>
     </row>
@@ -2594,7 +2597,7 @@
         <v>2012</v>
       </c>
       <c r="K23" s="2">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L23" s="1">
         <f>L22+C$5</f>
@@ -2609,7 +2612,7 @@
         <v>198960.99999999994</v>
       </c>
       <c r="Q23" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2244.333333333343</v>
       </c>
     </row>
@@ -2623,8 +2626,8 @@
       <c r="J24">
         <v>2013</v>
       </c>
-      <c r="K24">
-        <v>23</v>
+      <c r="K24" s="3">
+        <v>24</v>
       </c>
       <c r="L24" s="1">
         <f>L23+C$6</f>
@@ -2639,7 +2642,7 @@
         <v>199342.6666666666</v>
       </c>
       <c r="Q24" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>381.66666666665697</v>
       </c>
     </row>
@@ -2653,8 +2656,8 @@
       <c r="J25">
         <v>2014</v>
       </c>
-      <c r="K25">
-        <v>24</v>
+      <c r="K25" s="3">
+        <v>25</v>
       </c>
       <c r="L25" s="1">
         <f>L24+C$6</f>
@@ -2669,7 +2672,7 @@
         <v>199724.33333333326</v>
       </c>
       <c r="Q25" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>381.66666666665697</v>
       </c>
     </row>
@@ -2683,8 +2686,8 @@
       <c r="J26">
         <v>2015</v>
       </c>
-      <c r="K26">
-        <v>25</v>
+      <c r="K26" s="3">
+        <v>26</v>
       </c>
       <c r="L26" s="1">
         <f t="shared" ref="L26:L29" si="8">L25+C$6</f>
@@ -2699,7 +2702,7 @@
         <v>200105.99999999991</v>
       </c>
       <c r="Q26" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>381.66666666665697</v>
       </c>
     </row>
@@ -2710,8 +2713,8 @@
       <c r="J27">
         <v>2016</v>
       </c>
-      <c r="K27">
-        <v>26</v>
+      <c r="K27" s="3">
+        <v>27</v>
       </c>
       <c r="L27" s="1">
         <f t="shared" si="8"/>
@@ -2726,7 +2729,7 @@
         <v>200487.66666666657</v>
       </c>
       <c r="Q27" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>381.66666666665697</v>
       </c>
     </row>
@@ -2734,8 +2737,8 @@
       <c r="J28">
         <v>2017</v>
       </c>
-      <c r="K28">
-        <v>27</v>
+      <c r="K28" s="3">
+        <v>28</v>
       </c>
       <c r="L28" s="1">
         <f t="shared" si="8"/>
@@ -2750,7 +2753,7 @@
         <v>200869.33333333323</v>
       </c>
       <c r="Q28" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>381.66666666665697</v>
       </c>
     </row>
@@ -2762,7 +2765,7 @@
         <v>2018</v>
       </c>
       <c r="K29" s="2">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="L29" s="1">
         <f t="shared" si="8"/>
@@ -2777,7 +2780,7 @@
         <v>201250.99999999988</v>
       </c>
       <c r="Q29" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>381.66666666665697</v>
       </c>
     </row>
@@ -2785,11 +2788,13 @@
       <c r="A30" t="s">
         <v>3</v>
       </c>
+      <c r="K30" s="3"/>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>4</v>
       </c>
+      <c r="K31" s="3"/>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" t="s">

</xml_diff>